<commit_message>
sample table pasting; barcodes can be matched to samples based on primer plate + position
</commit_message>
<xml_diff>
--- a/barcodes/data/samples1.xlsx
+++ b/barcodes/data/samples1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyoungblut/ownCloud/Ley_lab/dev/R/shiny/RTecanFluentShiny/barcodes/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyoungblut/dev/R/RTecanFluentShiny/barcodes/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="18480" yWindow="3760" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
-  <si>
-    <t>#SampleID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
   <si>
     <t>Poop1</t>
   </si>
@@ -59,36 +56,12 @@
     <t>DNAx_blank</t>
   </si>
   <si>
-    <t>PCR_positive</t>
-  </si>
-  <si>
-    <t>PCR_negative</t>
-  </si>
-  <si>
-    <t>TECAN_sample_labware</t>
-  </si>
-  <si>
     <t>TECAN_sample_location</t>
   </si>
   <si>
-    <t>96 Well[001]</t>
-  </si>
-  <si>
-    <t>micro15[004]</t>
-  </si>
-  <si>
-    <t>micro15[005]</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>PCR water control (water in Tube 5)</t>
-  </si>
-  <si>
-    <t>Mock community (DNA in Tube 4)</t>
-  </si>
-  <si>
     <t>Tissue3</t>
   </si>
   <si>
@@ -104,7 +77,25 @@
     <t>DNA extraction blank</t>
   </si>
   <si>
-    <t>TECAN_sample_rxn_volume</t>
+    <t>TECAN_primer_labware_name</t>
+  </si>
+  <si>
+    <t>TECAN_primer_target_position</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>TECAN_sample_labware_name</t>
+  </si>
+  <si>
+    <t>Sample plate 1</t>
+  </si>
+  <si>
+    <t>N7-S5_1</t>
+  </si>
+  <si>
+    <t>N7-S5_2</t>
   </si>
 </sst>
 </file>
@@ -518,273 +509,277 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" customWidth="1"/>
+    <col min="3" max="5" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7">
+        <v>96</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
         <v>15</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>